<commit_message>
Chart class is changed to Metrics generation and add path in to properities file
</commit_message>
<xml_diff>
--- a/iTF/keywords/KeywordDriver.xlsx
+++ b/iTF/keywords/KeywordDriver.xlsx
@@ -43,9 +43,6 @@
     <t>#</t>
   </si>
   <si>
-    <t>Test description</t>
-  </si>
-  <si>
     <t>Run</t>
   </si>
   <si>
@@ -58,10 +55,13 @@
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>Userprofile</t>
-  </si>
-  <si>
-    <t>Usermodule</t>
+    <t>TestcasesbyModule</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Refering Modules Filename</t>
   </si>
 </sst>
 </file>
@@ -533,7 +533,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,13 +548,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -562,13 +562,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -591,7 +591,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>